<commit_message>
organized folders and loaded all games
</commit_message>
<xml_diff>
--- a/Colonizer Main/GameBoards.xlsx
+++ b/Colonizer Main/GameBoards.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10314"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kennethhsu/Google Drive/Hsu Family/Kenneth Hsu/Projects/Colonizer/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kennethhsu/Google Drive/Hsu Family/Kenneth Hsu/Projects/Colonizer/Github/Colonizer Main/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D35E7B1A-49DF-1547-9CD8-82347C12F808}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E0FBCFF-804B-2148-8507-11D8FAC31FA2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{ECD0B745-F889-C448-A747-C36281352244}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="38">
   <si>
     <t>Game</t>
   </si>
@@ -135,7 +135,10 @@
     <t>"5" Starting Location Offset</t>
   </si>
   <si>
-    <t>ClockwiseDiceSetup</t>
+    <t>ClockwiseDice</t>
+  </si>
+  <si>
+    <t>"sheep"</t>
   </si>
 </sst>
 </file>
@@ -496,10 +499,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B0F4AA2-A4EF-0047-9E07-AE4E15987399}">
-  <dimension ref="A1:AE7"/>
+  <dimension ref="A1:AE22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AA4" sqref="AA4"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="AE23" sqref="AE23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1176,8 +1179,1438 @@
         <v>0</v>
       </c>
     </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I8" t="s">
+        <v>10</v>
+      </c>
+      <c r="J8" t="s">
+        <v>11</v>
+      </c>
+      <c r="K8" t="s">
+        <v>10</v>
+      </c>
+      <c r="L8" t="s">
+        <v>13</v>
+      </c>
+      <c r="M8" t="s">
+        <v>15</v>
+      </c>
+      <c r="N8" t="s">
+        <v>13</v>
+      </c>
+      <c r="O8" t="s">
+        <v>11</v>
+      </c>
+      <c r="P8" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>12</v>
+      </c>
+      <c r="R8" t="s">
+        <v>10</v>
+      </c>
+      <c r="S8" t="s">
+        <v>11</v>
+      </c>
+      <c r="T8" t="s">
+        <v>13</v>
+      </c>
+      <c r="U8" t="s">
+        <v>11</v>
+      </c>
+      <c r="V8" t="s">
+        <v>10</v>
+      </c>
+      <c r="W8" t="s">
+        <v>12</v>
+      </c>
+      <c r="X8" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>14</v>
+      </c>
+      <c r="AC8" t="s">
+        <v>12</v>
+      </c>
+      <c r="AD8">
+        <v>6</v>
+      </c>
+      <c r="AE8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" t="s">
+        <v>12</v>
+      </c>
+      <c r="I9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K9" t="s">
+        <v>10</v>
+      </c>
+      <c r="L9" t="s">
+        <v>11</v>
+      </c>
+      <c r="M9" t="s">
+        <v>15</v>
+      </c>
+      <c r="N9" t="s">
+        <v>13</v>
+      </c>
+      <c r="O9" t="s">
+        <v>10</v>
+      </c>
+      <c r="P9" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>15</v>
+      </c>
+      <c r="R9" t="s">
+        <v>11</v>
+      </c>
+      <c r="S9" t="s">
+        <v>14</v>
+      </c>
+      <c r="T9" t="s">
+        <v>14</v>
+      </c>
+      <c r="U9" t="s">
+        <v>12</v>
+      </c>
+      <c r="V9" t="s">
+        <v>11</v>
+      </c>
+      <c r="W9" t="s">
+        <v>10</v>
+      </c>
+      <c r="X9" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>15</v>
+      </c>
+      <c r="AC9" t="s">
+        <v>14</v>
+      </c>
+      <c r="AD9">
+        <v>4</v>
+      </c>
+      <c r="AE9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" t="s">
+        <v>10</v>
+      </c>
+      <c r="I10" t="s">
+        <v>10</v>
+      </c>
+      <c r="J10" t="s">
+        <v>12</v>
+      </c>
+      <c r="K10" t="s">
+        <v>10</v>
+      </c>
+      <c r="L10" t="s">
+        <v>10</v>
+      </c>
+      <c r="M10" t="s">
+        <v>13</v>
+      </c>
+      <c r="N10" t="s">
+        <v>15</v>
+      </c>
+      <c r="O10" t="s">
+        <v>13</v>
+      </c>
+      <c r="P10" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>14</v>
+      </c>
+      <c r="R10" t="s">
+        <v>14</v>
+      </c>
+      <c r="S10" t="s">
+        <v>11</v>
+      </c>
+      <c r="T10" t="s">
+        <v>15</v>
+      </c>
+      <c r="U10" t="s">
+        <v>13</v>
+      </c>
+      <c r="V10" t="s">
+        <v>10</v>
+      </c>
+      <c r="W10" t="s">
+        <v>14</v>
+      </c>
+      <c r="X10" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>11</v>
+      </c>
+      <c r="AC10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AD10">
+        <v>6</v>
+      </c>
+      <c r="AE10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" t="s">
+        <v>12</v>
+      </c>
+      <c r="H11" t="s">
+        <v>10</v>
+      </c>
+      <c r="I11" t="s">
+        <v>11</v>
+      </c>
+      <c r="J11" t="s">
+        <v>13</v>
+      </c>
+      <c r="K11" t="s">
+        <v>11</v>
+      </c>
+      <c r="L11" t="s">
+        <v>15</v>
+      </c>
+      <c r="M11" t="s">
+        <v>13</v>
+      </c>
+      <c r="N11" t="s">
+        <v>14</v>
+      </c>
+      <c r="O11" t="s">
+        <v>14</v>
+      </c>
+      <c r="P11" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>10</v>
+      </c>
+      <c r="R11" t="s">
+        <v>15</v>
+      </c>
+      <c r="S11" t="s">
+        <v>15</v>
+      </c>
+      <c r="T11" t="s">
+        <v>15</v>
+      </c>
+      <c r="U11" t="s">
+        <v>12</v>
+      </c>
+      <c r="V11" t="s">
+        <v>13</v>
+      </c>
+      <c r="W11" t="s">
+        <v>14</v>
+      </c>
+      <c r="X11" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>11</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>15</v>
+      </c>
+      <c r="AC11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AD11">
+        <v>4</v>
+      </c>
+      <c r="AE11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" t="s">
+        <v>11</v>
+      </c>
+      <c r="H12" t="s">
+        <v>10</v>
+      </c>
+      <c r="I12" t="s">
+        <v>10</v>
+      </c>
+      <c r="J12" t="s">
+        <v>12</v>
+      </c>
+      <c r="K12" t="s">
+        <v>15</v>
+      </c>
+      <c r="L12" t="s">
+        <v>10</v>
+      </c>
+      <c r="M12" t="s">
+        <v>14</v>
+      </c>
+      <c r="N12" t="s">
+        <v>11</v>
+      </c>
+      <c r="O12" t="s">
+        <v>13</v>
+      </c>
+      <c r="P12" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>15</v>
+      </c>
+      <c r="R12" t="s">
+        <v>14</v>
+      </c>
+      <c r="S12" t="s">
+        <v>13</v>
+      </c>
+      <c r="T12" t="s">
+        <v>10</v>
+      </c>
+      <c r="U12" t="s">
+        <v>13</v>
+      </c>
+      <c r="V12" t="s">
+        <v>11</v>
+      </c>
+      <c r="W12" t="s">
+        <v>15</v>
+      </c>
+      <c r="X12" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA12" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB12" t="s">
+        <v>12</v>
+      </c>
+      <c r="AC12" t="s">
+        <v>12</v>
+      </c>
+      <c r="AD12">
+        <v>2</v>
+      </c>
+      <c r="AE12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H13" t="s">
+        <v>10</v>
+      </c>
+      <c r="I13" t="s">
+        <v>11</v>
+      </c>
+      <c r="J13" t="s">
+        <v>10</v>
+      </c>
+      <c r="K13" t="s">
+        <v>15</v>
+      </c>
+      <c r="L13" t="s">
+        <v>12</v>
+      </c>
+      <c r="M13" t="s">
+        <v>11</v>
+      </c>
+      <c r="N13" t="s">
+        <v>13</v>
+      </c>
+      <c r="O13" t="s">
+        <v>14</v>
+      </c>
+      <c r="P13" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>15</v>
+      </c>
+      <c r="R13" t="s">
+        <v>13</v>
+      </c>
+      <c r="S13" t="s">
+        <v>15</v>
+      </c>
+      <c r="T13" t="s">
+        <v>11</v>
+      </c>
+      <c r="U13" t="s">
+        <v>10</v>
+      </c>
+      <c r="V13" t="s">
+        <v>12</v>
+      </c>
+      <c r="W13" t="s">
+        <v>11</v>
+      </c>
+      <c r="X13" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z13" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA13" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB13" t="s">
+        <v>12</v>
+      </c>
+      <c r="AC13" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD13">
+        <v>8</v>
+      </c>
+      <c r="AE13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" t="s">
+        <v>12</v>
+      </c>
+      <c r="H14" t="s">
+        <v>15</v>
+      </c>
+      <c r="I14" t="s">
+        <v>13</v>
+      </c>
+      <c r="J14" t="s">
+        <v>11</v>
+      </c>
+      <c r="K14" t="s">
+        <v>14</v>
+      </c>
+      <c r="L14" t="s">
+        <v>13</v>
+      </c>
+      <c r="M14" t="s">
+        <v>10</v>
+      </c>
+      <c r="N14" t="s">
+        <v>15</v>
+      </c>
+      <c r="O14" t="s">
+        <v>15</v>
+      </c>
+      <c r="P14" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>11</v>
+      </c>
+      <c r="R14" t="s">
+        <v>10</v>
+      </c>
+      <c r="S14" t="s">
+        <v>14</v>
+      </c>
+      <c r="T14" t="s">
+        <v>11</v>
+      </c>
+      <c r="U14" t="s">
+        <v>14</v>
+      </c>
+      <c r="V14" t="s">
+        <v>12</v>
+      </c>
+      <c r="W14" t="s">
+        <v>15</v>
+      </c>
+      <c r="X14" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z14" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA14" t="s">
+        <v>10</v>
+      </c>
+      <c r="AB14" t="s">
+        <v>12</v>
+      </c>
+      <c r="AC14" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD14">
+        <v>6</v>
+      </c>
+      <c r="AE14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" t="s">
+        <v>12</v>
+      </c>
+      <c r="G15" t="s">
+        <v>10</v>
+      </c>
+      <c r="H15" t="s">
+        <v>10</v>
+      </c>
+      <c r="I15" t="s">
+        <v>11</v>
+      </c>
+      <c r="J15" t="s">
+        <v>15</v>
+      </c>
+      <c r="K15" t="s">
+        <v>14</v>
+      </c>
+      <c r="L15" t="s">
+        <v>14</v>
+      </c>
+      <c r="M15" t="s">
+        <v>13</v>
+      </c>
+      <c r="N15" t="s">
+        <v>13</v>
+      </c>
+      <c r="O15" t="s">
+        <v>11</v>
+      </c>
+      <c r="P15" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>14</v>
+      </c>
+      <c r="R15" t="s">
+        <v>15</v>
+      </c>
+      <c r="S15" t="s">
+        <v>15</v>
+      </c>
+      <c r="T15" t="s">
+        <v>11</v>
+      </c>
+      <c r="U15" t="s">
+        <v>12</v>
+      </c>
+      <c r="V15" t="s">
+        <v>12</v>
+      </c>
+      <c r="W15" t="s">
+        <v>12</v>
+      </c>
+      <c r="X15" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA15" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB15" t="s">
+        <v>11</v>
+      </c>
+      <c r="AC15" t="s">
+        <v>10</v>
+      </c>
+      <c r="AD15">
+        <v>6</v>
+      </c>
+      <c r="AE15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" t="s">
+        <v>15</v>
+      </c>
+      <c r="G16" t="s">
+        <v>11</v>
+      </c>
+      <c r="H16" t="s">
+        <v>10</v>
+      </c>
+      <c r="I16" t="s">
+        <v>13</v>
+      </c>
+      <c r="J16" t="s">
+        <v>11</v>
+      </c>
+      <c r="K16" t="s">
+        <v>15</v>
+      </c>
+      <c r="L16" t="s">
+        <v>15</v>
+      </c>
+      <c r="M16" t="s">
+        <v>12</v>
+      </c>
+      <c r="N16" t="s">
+        <v>14</v>
+      </c>
+      <c r="O16" t="s">
+        <v>14</v>
+      </c>
+      <c r="P16" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>10</v>
+      </c>
+      <c r="R16" t="s">
+        <v>13</v>
+      </c>
+      <c r="S16" t="s">
+        <v>11</v>
+      </c>
+      <c r="T16" t="s">
+        <v>10</v>
+      </c>
+      <c r="U16" t="s">
+        <v>15</v>
+      </c>
+      <c r="V16" t="s">
+        <v>10</v>
+      </c>
+      <c r="W16" t="s">
+        <v>11</v>
+      </c>
+      <c r="X16" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z16" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA16" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB16" t="s">
+        <v>12</v>
+      </c>
+      <c r="AC16" t="s">
+        <v>12</v>
+      </c>
+      <c r="AD16">
+        <v>2</v>
+      </c>
+      <c r="AE16" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17" t="s">
+        <v>12</v>
+      </c>
+      <c r="G17" t="s">
+        <v>15</v>
+      </c>
+      <c r="H17" t="s">
+        <v>13</v>
+      </c>
+      <c r="I17" t="s">
+        <v>10</v>
+      </c>
+      <c r="J17" t="s">
+        <v>15</v>
+      </c>
+      <c r="K17" t="s">
+        <v>14</v>
+      </c>
+      <c r="L17" t="s">
+        <v>14</v>
+      </c>
+      <c r="M17" t="s">
+        <v>14</v>
+      </c>
+      <c r="N17" t="s">
+        <v>13</v>
+      </c>
+      <c r="O17" t="s">
+        <v>10</v>
+      </c>
+      <c r="P17" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>11</v>
+      </c>
+      <c r="R17" t="s">
+        <v>11</v>
+      </c>
+      <c r="S17" t="s">
+        <v>15</v>
+      </c>
+      <c r="T17" t="s">
+        <v>11</v>
+      </c>
+      <c r="U17" t="s">
+        <v>12</v>
+      </c>
+      <c r="V17" t="s">
+        <v>11</v>
+      </c>
+      <c r="W17" t="s">
+        <v>12</v>
+      </c>
+      <c r="X17" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z17" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA17" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB17" t="s">
+        <v>15</v>
+      </c>
+      <c r="AC17" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD17">
+        <v>4</v>
+      </c>
+      <c r="AE17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18" t="s">
+        <v>11</v>
+      </c>
+      <c r="F18" t="s">
+        <v>13</v>
+      </c>
+      <c r="G18" t="s">
+        <v>12</v>
+      </c>
+      <c r="H18" t="s">
+        <v>13</v>
+      </c>
+      <c r="I18" t="s">
+        <v>10</v>
+      </c>
+      <c r="J18" t="s">
+        <v>15</v>
+      </c>
+      <c r="K18" t="s">
+        <v>13</v>
+      </c>
+      <c r="L18" t="s">
+        <v>14</v>
+      </c>
+      <c r="M18" t="s">
+        <v>10</v>
+      </c>
+      <c r="N18" t="s">
+        <v>15</v>
+      </c>
+      <c r="O18" t="s">
+        <v>15</v>
+      </c>
+      <c r="P18" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>11</v>
+      </c>
+      <c r="R18" t="s">
+        <v>11</v>
+      </c>
+      <c r="S18" t="s">
+        <v>10</v>
+      </c>
+      <c r="T18" t="s">
+        <v>10</v>
+      </c>
+      <c r="U18" t="s">
+        <v>11</v>
+      </c>
+      <c r="V18" t="s">
+        <v>12</v>
+      </c>
+      <c r="W18" t="s">
+        <v>13</v>
+      </c>
+      <c r="X18" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z18" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA18" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB18" t="s">
+        <v>15</v>
+      </c>
+      <c r="AC18" t="s">
+        <v>12</v>
+      </c>
+      <c r="AD18">
+        <v>10</v>
+      </c>
+      <c r="AE18" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" t="s">
+        <v>13</v>
+      </c>
+      <c r="F19" t="s">
+        <v>14</v>
+      </c>
+      <c r="G19" t="s">
+        <v>13</v>
+      </c>
+      <c r="H19" t="s">
+        <v>13</v>
+      </c>
+      <c r="I19" t="s">
+        <v>11</v>
+      </c>
+      <c r="J19" t="s">
+        <v>15</v>
+      </c>
+      <c r="K19" t="s">
+        <v>14</v>
+      </c>
+      <c r="L19" t="s">
+        <v>11</v>
+      </c>
+      <c r="M19" t="s">
+        <v>15</v>
+      </c>
+      <c r="N19" t="s">
+        <v>10</v>
+      </c>
+      <c r="O19" t="s">
+        <v>11</v>
+      </c>
+      <c r="P19" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>15</v>
+      </c>
+      <c r="R19" t="s">
+        <v>10</v>
+      </c>
+      <c r="S19" t="s">
+        <v>14</v>
+      </c>
+      <c r="T19" t="s">
+        <v>10</v>
+      </c>
+      <c r="U19" t="s">
+        <v>13</v>
+      </c>
+      <c r="V19" t="s">
+        <v>11</v>
+      </c>
+      <c r="W19" t="s">
+        <v>12</v>
+      </c>
+      <c r="X19" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y19" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z19" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA19" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB19" t="s">
+        <v>12</v>
+      </c>
+      <c r="AC19" t="s">
+        <v>15</v>
+      </c>
+      <c r="AD19">
+        <v>0</v>
+      </c>
+      <c r="AE19" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20" t="s">
+        <v>10</v>
+      </c>
+      <c r="G20" t="s">
+        <v>13</v>
+      </c>
+      <c r="H20" t="s">
+        <v>10</v>
+      </c>
+      <c r="I20" t="s">
+        <v>14</v>
+      </c>
+      <c r="J20" t="s">
+        <v>13</v>
+      </c>
+      <c r="K20" t="s">
+        <v>15</v>
+      </c>
+      <c r="L20" t="s">
+        <v>15</v>
+      </c>
+      <c r="M20" t="s">
+        <v>11</v>
+      </c>
+      <c r="N20" t="s">
+        <v>11</v>
+      </c>
+      <c r="O20" t="s">
+        <v>13</v>
+      </c>
+      <c r="P20" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>10</v>
+      </c>
+      <c r="R20" t="s">
+        <v>15</v>
+      </c>
+      <c r="S20" t="s">
+        <v>15</v>
+      </c>
+      <c r="T20" t="s">
+        <v>14</v>
+      </c>
+      <c r="U20" t="s">
+        <v>12</v>
+      </c>
+      <c r="V20" t="s">
+        <v>14</v>
+      </c>
+      <c r="W20" t="s">
+        <v>15</v>
+      </c>
+      <c r="X20" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y20" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z20" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA20" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB20" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC20" t="s">
+        <v>12</v>
+      </c>
+      <c r="AD20">
+        <v>6</v>
+      </c>
+      <c r="AE20" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" t="s">
+        <v>11</v>
+      </c>
+      <c r="F21" t="s">
+        <v>12</v>
+      </c>
+      <c r="G21" t="s">
+        <v>15</v>
+      </c>
+      <c r="H21" t="s">
+        <v>13</v>
+      </c>
+      <c r="I21" t="s">
+        <v>15</v>
+      </c>
+      <c r="J21" t="s">
+        <v>10</v>
+      </c>
+      <c r="K21" t="s">
+        <v>15</v>
+      </c>
+      <c r="L21" t="s">
+        <v>14</v>
+      </c>
+      <c r="M21" t="s">
+        <v>14</v>
+      </c>
+      <c r="N21" t="s">
+        <v>10</v>
+      </c>
+      <c r="O21" t="s">
+        <v>11</v>
+      </c>
+      <c r="P21" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>11</v>
+      </c>
+      <c r="R21" t="s">
+        <v>13</v>
+      </c>
+      <c r="S21" t="s">
+        <v>10</v>
+      </c>
+      <c r="T21" t="s">
+        <v>15</v>
+      </c>
+      <c r="U21" t="s">
+        <v>12</v>
+      </c>
+      <c r="V21" t="s">
+        <v>12</v>
+      </c>
+      <c r="W21" t="s">
+        <v>15</v>
+      </c>
+      <c r="X21" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y21" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z21" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA21" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB21" t="s">
+        <v>12</v>
+      </c>
+      <c r="AC21" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD21">
+        <v>10</v>
+      </c>
+      <c r="AE21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" t="s">
+        <v>11</v>
+      </c>
+      <c r="F22" t="s">
+        <v>15</v>
+      </c>
+      <c r="G22" t="s">
+        <v>11</v>
+      </c>
+      <c r="H22" t="s">
+        <v>10</v>
+      </c>
+      <c r="I22" t="s">
+        <v>13</v>
+      </c>
+      <c r="J22" t="s">
+        <v>15</v>
+      </c>
+      <c r="K22" t="s">
+        <v>11</v>
+      </c>
+      <c r="L22" t="s">
+        <v>10</v>
+      </c>
+      <c r="M22" t="s">
+        <v>10</v>
+      </c>
+      <c r="N22" t="s">
+        <v>15</v>
+      </c>
+      <c r="O22" t="s">
+        <v>14</v>
+      </c>
+      <c r="P22" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>14</v>
+      </c>
+      <c r="R22" t="s">
+        <v>13</v>
+      </c>
+      <c r="S22" t="s">
+        <v>12</v>
+      </c>
+      <c r="T22" t="s">
+        <v>14</v>
+      </c>
+      <c r="U22" t="s">
+        <v>15</v>
+      </c>
+      <c r="V22" t="s">
+        <v>12</v>
+      </c>
+      <c r="W22" t="s">
+        <v>12</v>
+      </c>
+      <c r="X22" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y22" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z22" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA22" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB22" t="s">
+        <v>11</v>
+      </c>
+      <c r="AC22" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD22">
+        <v>6</v>
+      </c>
+      <c r="AE22" t="b">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:AC20 B22:AC1048576 B21:Z21 AB21:AC21" xr:uid="{BD4759BE-4F06-9042-9E94-B9EC5A548EFC}">
+      <formula1>"wood,brick,sheep,wheat,rock,desert"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
able to calculate ranking by tiles available and probability
</commit_message>
<xml_diff>
--- a/Colonizer Main/GameBoards.xlsx
+++ b/Colonizer Main/GameBoards.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kennethhsu/Google Drive/Hsu Family/Kenneth Hsu/Projects/Colonizer/Github/Colonizer Main/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E0FBCFF-804B-2148-8507-11D8FAC31FA2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{208CDE3A-1452-3145-A28E-DF11F9ADE1DD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{ECD0B745-F889-C448-A747-C36281352244}"/>
+    <workbookView xWindow="-46840" yWindow="-4180" windowWidth="33600" windowHeight="20500" xr2:uid="{ECD0B745-F889-C448-A747-C36281352244}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="37">
   <si>
     <t>Game</t>
   </si>
@@ -136,9 +136,6 @@
   </si>
   <si>
     <t>ClockwiseDice</t>
-  </si>
-  <si>
-    <t>"sheep"</t>
   </si>
 </sst>
 </file>
@@ -501,8 +498,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B0F4AA2-A4EF-0047-9E07-AE4E15987399}">
   <dimension ref="A1:AE22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="AE23" sqref="AE23"/>
+    <sheetView tabSelected="1" zoomScale="212" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1279,7 +1276,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="C9" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
implemented dice statistics (partially)
</commit_message>
<xml_diff>
--- a/Colonizer Main/GameBoards.xlsx
+++ b/Colonizer Main/GameBoards.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kennethhsu/Google Drive/Hsu Family/Kenneth Hsu/Projects/Colonizer/Github/Colonizer Main/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{208CDE3A-1452-3145-A28E-DF11F9ADE1DD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DF11921-D931-6A47-A2A8-3F4900BED802}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-46840" yWindow="-4180" windowWidth="33600" windowHeight="20500" xr2:uid="{ECD0B745-F889-C448-A747-C36281352244}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{ECD0B745-F889-C448-A747-C36281352244}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="37">
   <si>
     <t>Game</t>
   </si>
@@ -57,9 +57,6 @@
     <t>Port 9</t>
   </si>
   <si>
-    <t>wood</t>
-  </si>
-  <si>
     <t>wheat</t>
   </si>
   <si>
@@ -136,6 +133,9 @@
   </si>
   <si>
     <t>ClockwiseDice</t>
+  </si>
+  <si>
+    <t>lumber</t>
   </si>
 </sst>
 </file>
@@ -496,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B0F4AA2-A4EF-0047-9E07-AE4E15987399}">
-  <dimension ref="A1:AE22"/>
+  <dimension ref="A1:AE25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="212" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -516,61 +516,61 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
         <v>16</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>17</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>18</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>19</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>20</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>21</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>22</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>23</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>24</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>25</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>26</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>27</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>28</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>29</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>30</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>31</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>32</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>33</v>
-      </c>
-      <c r="T1" t="s">
-        <v>34</v>
       </c>
       <c r="U1" t="s">
         <v>1</v>
@@ -600,10 +600,10 @@
         <v>9</v>
       </c>
       <c r="AD1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE1" t="s">
         <v>35</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.2">
@@ -611,88 +611,88 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J2" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="K2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N2" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="O2" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="P2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Q2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="R2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="S2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="T2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="U2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="V2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="W2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="X2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Y2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="Z2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="AA2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="AB2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AC2" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="AD2">
         <v>0</v>
@@ -706,88 +706,88 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J3" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="K3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="L3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="N3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="O3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="P3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Q3" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="R3" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="S3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="T3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="U3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="V3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="W3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="X3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Y3" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="Z3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AA3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AB3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="AC3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AD3">
         <v>0</v>
@@ -801,88 +801,88 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F4" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="G4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="L4" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="M4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="N4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="O4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="P4" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="Q4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="R4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="S4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="T4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="U4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="V4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="W4" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="X4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="Y4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Z4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="AA4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AB4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AC4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AD4">
         <v>0</v>
@@ -896,88 +896,88 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F5" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="G5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="L5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="M5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="O5" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="P5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="Q5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="R5" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="S5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="T5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="U5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="V5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="W5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="X5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Y5" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="Z5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AA5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AB5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AC5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="AD5">
         <v>0</v>
@@ -991,88 +991,88 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J6" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="K6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L6" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="M6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="N6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="O6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="P6" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="Q6" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="R6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="S6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="T6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="U6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="V6" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="W6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="X6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Y6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Z6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AA6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AB6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AC6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AD6">
         <v>0</v>
@@ -1086,88 +1086,88 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D7" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="E7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K7" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="L7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="N7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="O7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="P7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Q7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="R7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="S7" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="T7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="U7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="V7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="W7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="X7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="Y7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="Z7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AA7" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="AB7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AC7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="AD7">
         <v>2</v>
@@ -1181,88 +1181,88 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G8" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="H8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I8" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="J8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K8" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="L8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="M8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="O8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="P8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="R8" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="S8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="T8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="U8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="V8" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="W8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="X8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="Y8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="Z8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AA8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="AB8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="AC8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AD8">
         <v>6</v>
@@ -1276,88 +1276,88 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E9" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="F9" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="G9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K9" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="L9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="O9" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="P9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="Q9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="R9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="S9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="T9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="U9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="V9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="W9" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="X9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="Y9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="Z9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="AA9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AB9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AC9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="AD9">
         <v>4</v>
@@ -1371,88 +1371,88 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H10" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="I10" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="J10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K10" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="L10" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="M10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="N10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="O10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="P10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Q10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="R10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="S10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="T10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="U10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="V10" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="W10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="X10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="Y10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="Z10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AA10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AB10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="AC10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AD10">
         <v>6</v>
@@ -1466,88 +1466,88 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="C11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F11" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="G11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H11" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="I11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="N11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="O11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="P11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Q11" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="R11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="S11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="T11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="U11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="V11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="W11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="X11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="Y11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="Z11" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="AA11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="AB11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AC11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AD11">
         <v>4</v>
@@ -1561,88 +1561,88 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H12" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="I12" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="J12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L12" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="M12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="N12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="O12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="P12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="R12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="S12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="T12" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="U12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="V12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="W12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="X12" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="Y12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="Z12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AA12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="AB12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AC12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AD12">
         <v>2</v>
@@ -1656,88 +1656,88 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E13" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="F13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G13" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="H13" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="I13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J13" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="K13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="M13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="N13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="O13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="P13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Q13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="R13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="S13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="T13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="U13" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="V13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="W13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="X13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="Y13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="Z13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="AA13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AB13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AC13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="AD13">
         <v>8</v>
@@ -1751,88 +1751,88 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E14" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="F14" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="G14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="M14" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="N14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="O14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="P14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="Q14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="R14" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="S14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="T14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="U14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="V14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="W14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="X14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="Y14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="Z14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="AA14" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="AB14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AC14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="AD14">
         <v>6</v>
@@ -1846,88 +1846,88 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="C15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E15" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="F15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G15" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="H15" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="I15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="M15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="N15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="O15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="P15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="Q15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="R15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="S15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="T15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="U15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="V15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="W15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="X15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Y15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="Z15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="AA15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AB15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="AC15" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="AD15">
         <v>6</v>
@@ -1941,88 +1941,88 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C16" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="D16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H16" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="I16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="N16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="O16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="P16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="Q16" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="R16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="S16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="T16" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="U16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="V16" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="W16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="X16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="Y16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="Z16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="AA16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AB16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AC16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AD16">
         <v>2</v>
@@ -2036,88 +2036,88 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C17" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="D17" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="E17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I17" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="J17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="M17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="N17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="O17" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="P17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="Q17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="R17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="S17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="T17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="U17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="V17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="W17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="X17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Y17" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="Z17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AA17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AB17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AC17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="AD17">
         <v>4</v>
@@ -2131,88 +2131,88 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I18" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="J18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="L18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="M18" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="N18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="O18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="P18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="R18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="S18" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="T18" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="U18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="V18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="W18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="X18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="Y18" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="Z18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AA18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="AB18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AC18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AD18">
         <v>10</v>
@@ -2226,88 +2226,88 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D19" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="E19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N19" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="O19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="P19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Q19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="R19" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="S19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="T19" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="U19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="V19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="W19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="X19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="Y19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Z19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AA19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="AB19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AC19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AD19">
         <v>0</v>
@@ -2321,88 +2321,88 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F20" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="G20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H20" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="I20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="N20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="O20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="P20" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="Q20" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="R20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="S20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="T20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="U20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="V20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="W20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="X20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Y20" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="Z20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AA20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AB20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="AC20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AD20">
         <v>6</v>
@@ -2416,88 +2416,88 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D21" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="E21" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F21" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H21" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J21" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="K21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="M21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="N21" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="O21" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="P21" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Q21" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="R21" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="S21" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="T21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="U21" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="V21" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="W21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="X21" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="Y21" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Z21" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AA21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="AB21" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AC21" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="AD21">
         <v>10</v>
@@ -2511,101 +2511,389 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D22" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="E22" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G22" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H22" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="I22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K22" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L22" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="M22" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="N22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="O22" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="P22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="Q22" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="R22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="S22" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="T22" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="U22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="V22" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="W22" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="X22" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="Y22" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Z22" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="AA22" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AB22" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="AC22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="AD22">
         <v>6</v>
       </c>
       <c r="AE22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" t="s">
+        <v>14</v>
+      </c>
+      <c r="E23" t="s">
+        <v>12</v>
+      </c>
+      <c r="F23" t="s">
+        <v>13</v>
+      </c>
+      <c r="G23" t="s">
+        <v>13</v>
+      </c>
+      <c r="H23" t="s">
+        <v>36</v>
+      </c>
+      <c r="I23" t="s">
+        <v>10</v>
+      </c>
+      <c r="J23" t="s">
+        <v>13</v>
+      </c>
+      <c r="K23" t="s">
+        <v>12</v>
+      </c>
+      <c r="L23" t="s">
+        <v>14</v>
+      </c>
+      <c r="M23" t="s">
+        <v>14</v>
+      </c>
+      <c r="N23" t="s">
+        <v>10</v>
+      </c>
+      <c r="O23" t="s">
+        <v>10</v>
+      </c>
+      <c r="P23" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>11</v>
+      </c>
+      <c r="R23" t="s">
+        <v>36</v>
+      </c>
+      <c r="S23" t="s">
+        <v>36</v>
+      </c>
+      <c r="T23" t="s">
+        <v>10</v>
+      </c>
+      <c r="U23" t="s">
+        <v>11</v>
+      </c>
+      <c r="V23" t="s">
+        <v>12</v>
+      </c>
+      <c r="W23" t="s">
+        <v>11</v>
+      </c>
+      <c r="X23" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y23" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z23" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA23" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB23" t="s">
+        <v>10</v>
+      </c>
+      <c r="AC23" t="s">
+        <v>14</v>
+      </c>
+      <c r="AD23">
+        <v>10</v>
+      </c>
+      <c r="AE23" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24" t="s">
+        <v>13</v>
+      </c>
+      <c r="D24" t="s">
+        <v>13</v>
+      </c>
+      <c r="E24" t="s">
+        <v>10</v>
+      </c>
+      <c r="F24" t="s">
+        <v>12</v>
+      </c>
+      <c r="G24" t="s">
+        <v>36</v>
+      </c>
+      <c r="H24" t="s">
+        <v>13</v>
+      </c>
+      <c r="I24" t="s">
+        <v>36</v>
+      </c>
+      <c r="J24" t="s">
+        <v>12</v>
+      </c>
+      <c r="K24" t="s">
+        <v>36</v>
+      </c>
+      <c r="L24" t="s">
+        <v>10</v>
+      </c>
+      <c r="M24" t="s">
+        <v>14</v>
+      </c>
+      <c r="N24" t="s">
+        <v>14</v>
+      </c>
+      <c r="O24" t="s">
+        <v>14</v>
+      </c>
+      <c r="P24" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>14</v>
+      </c>
+      <c r="R24" t="s">
+        <v>10</v>
+      </c>
+      <c r="S24" t="s">
+        <v>10</v>
+      </c>
+      <c r="T24" t="s">
+        <v>11</v>
+      </c>
+      <c r="U24" t="s">
+        <v>11</v>
+      </c>
+      <c r="V24" t="s">
+        <v>11</v>
+      </c>
+      <c r="W24" t="s">
+        <v>14</v>
+      </c>
+      <c r="X24" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y24" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z24" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA24" t="s">
+        <v>11</v>
+      </c>
+      <c r="AB24" t="s">
+        <v>11</v>
+      </c>
+      <c r="AC24" t="s">
+        <v>10</v>
+      </c>
+      <c r="AD24">
+        <v>0</v>
+      </c>
+      <c r="AE24" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" t="s">
+        <v>13</v>
+      </c>
+      <c r="D25" t="s">
+        <v>14</v>
+      </c>
+      <c r="E25" t="s">
+        <v>36</v>
+      </c>
+      <c r="F25" t="s">
+        <v>14</v>
+      </c>
+      <c r="G25" t="s">
+        <v>36</v>
+      </c>
+      <c r="H25" t="s">
+        <v>13</v>
+      </c>
+      <c r="I25" t="s">
+        <v>14</v>
+      </c>
+      <c r="J25" t="s">
+        <v>11</v>
+      </c>
+      <c r="K25" t="s">
+        <v>12</v>
+      </c>
+      <c r="L25" t="s">
+        <v>14</v>
+      </c>
+      <c r="M25" t="s">
+        <v>12</v>
+      </c>
+      <c r="N25" t="s">
+        <v>10</v>
+      </c>
+      <c r="O25" t="s">
+        <v>10</v>
+      </c>
+      <c r="P25" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>10</v>
+      </c>
+      <c r="R25" t="s">
+        <v>36</v>
+      </c>
+      <c r="S25" t="s">
+        <v>13</v>
+      </c>
+      <c r="T25" t="s">
+        <v>12</v>
+      </c>
+      <c r="U25" t="s">
+        <v>11</v>
+      </c>
+      <c r="V25" t="s">
+        <v>11</v>
+      </c>
+      <c r="W25" t="s">
+        <v>14</v>
+      </c>
+      <c r="X25" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y25" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z25" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA25" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB25" t="s">
+        <v>11</v>
+      </c>
+      <c r="AC25" t="s">
+        <v>12</v>
+      </c>
+      <c r="AD25">
+        <v>0</v>
+      </c>
+      <c r="AE25" t="b">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:AC20 B22:AC1048576 B21:Z21 AB21:AC21" xr:uid="{BD4759BE-4F06-9042-9E94-B9EC5A548EFC}">
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:AC1" xr:uid="{BD4759BE-4F06-9042-9E94-B9EC5A548EFC}">
       <formula1>"wood,brick,sheep,wheat,rock,desert"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:AC1048576" xr:uid="{A9F2EF2F-3D9D-D34F-A577-210E4A6B9520}">
+      <formula1>"lumber,brick,sheep,wheat,rock,desert"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
started some work on development cards tracking
</commit_message>
<xml_diff>
--- a/Colonizer Main/GameBoards.xlsx
+++ b/Colonizer Main/GameBoards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kennethhsu/Google Drive/Hsu Family/Kenneth Hsu/Projects/Colonizer/Github/Colonizer Main/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7CD00B7-2934-6D49-8BC0-8AE38CDD4128}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F296166-75D9-8C41-B8C0-964C5EB5141A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{ECD0B745-F889-C448-A747-C36281352244}"/>
   </bookViews>
@@ -498,8 +498,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B0F4AA2-A4EF-0047-9E07-AE4E15987399}">
   <dimension ref="A1:AE25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="X27" sqref="X27"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F26" sqref="A26:XFD26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>